<commit_message>
change tables headers and fix reading issues of the database from the python file
</commit_message>
<xml_diff>
--- a/iPHAOS.xlsx
+++ b/iPHAOS.xlsx
@@ -48,8 +48,7 @@
     <t xml:space="preserve">Spectral resolution [nm]</t>
   </si>
   <si>
-    <t xml:space="preserve">Bandwidth-to-resolution
- ratio</t>
+    <t xml:space="preserve">Bandwidth-to-resolution ratio</t>
   </si>
   <si>
     <t xml:space="preserve">Dynamic range</t>
@@ -1715,8 +1714,8 @@
   </sheetPr>
   <dimension ref="A1:P268"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="193" zoomScaleNormal="193" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O48" activeCellId="0" sqref="A1:O48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="193" zoomScaleNormal="193" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5844,10 +5843,10 @@
   <dimension ref="A1:AMJ72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="193" zoomScaleNormal="193" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:O48"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.86"/>
@@ -8510,10 +8509,10 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="193" zoomScaleNormal="193" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="1" sqref="A1:O48 B63"/>
+      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.14"/>

</xml_diff>

<commit_message>
add momeni hosseini askari soltani adibi optics communications 2009 to the database
</commit_message>
<xml_diff>
--- a/iPHAOS.xlsx
+++ b/iPHAOS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="276">
   <si>
     <t xml:space="preserve">Spectral range</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t xml:space="preserve">Redding, B., Liew, S., Sarma, R. et al. Compact spectrometer based on a disordered photonic chip. Nature Photon 7, 746–751 (2013). https://doi.org/10.1038/nphoton.2013.190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 x 220 e-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babak Momeni, Ehsan Shah Hosseini, Murtaza Askari, Mohammad Soltani, Ali Adibi, Integrated photonic crystal spectrometers for sensing applications, Optics Communications, Volume 282, Issue 15, 2009</t>
   </si>
   <si>
     <t xml:space="preserve">Material</t>
@@ -972,11 +978,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
-    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -1300,7 +1305,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1461,7 +1466,7 @@
   <dimension ref="A1:O268"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O13" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O55" activeCellId="0" sqref="O55"/>
+      <selection pane="topLeft" activeCell="O50" activeCellId="0" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3330,9 +3335,7 @@
         <v>33.3333333333333</v>
       </c>
       <c r="I49" s="14"/>
-      <c r="J49" s="21" t="n">
-        <v>2.5E-005</v>
-      </c>
+      <c r="J49" s="21"/>
       <c r="K49" s="14"/>
       <c r="L49" s="14"/>
       <c r="M49" s="14" t="s">
@@ -3346,24 +3349,44 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="14" t="n">
+        <v>1560</v>
+      </c>
+      <c r="D50" s="14" t="n">
+        <v>1610</v>
+      </c>
+      <c r="E50" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="F50" s="14" t="n">
+        <v>1585</v>
+      </c>
       <c r="G50" s="14"/>
       <c r="H50" s="15" t="str">
         <f aca="false">IF(AND(E50&lt;&gt;0,G50&lt;&gt;0),E50/G50,"")</f>
         <v/>
       </c>
       <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
+      <c r="J50" s="14" t="s">
+        <v>103</v>
+      </c>
       <c r="K50" s="14"/>
       <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="19"/>
+      <c r="M50" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N50" s="14" t="n">
+        <v>2009</v>
+      </c>
+      <c r="O50" s="19" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="14"/>
@@ -5404,6 +5427,7 @@
     <hyperlink ref="O47" r:id="rId45" display="M. Muneeb, X. Chen, P. Verheyen, G. Lepage, S. Pathak, E. Ryckeboer, A. Malik, B. Kuyken, M. Nedeljkovic, J. Van Campenhout, G. Z. Mashanovich, and G. Roelkens, &quot;Demonstration of Silicon-on-insulator mid-infrared spectrometers operating at 3.8μm,&quot; Opt. Ex"/>
     <hyperlink ref="O48" r:id="rId46" display="J. Brouckaert, W. Bogaerts, S. Selvaraja, P. Dumon, R. Baets and D. Van Thourhout, &quot;Planar Concave Grating Demultiplexer With High Reflective Bragg Reflector Facets,&quot; in IEEE Photonics Technology Letters, vol. 20, no. 4, pp. 309-311, Feb.15, 2008, doi: 10"/>
     <hyperlink ref="O49" r:id="rId47" location="citeas" display="Redding, B., Liew, S., Sarma, R. et al. Compact spectrometer based on a disordered photonic chip. Nature Photon 7, 746–751 (2013). https://doi.org/10.1038/nphoton.2013.190"/>
+    <hyperlink ref="O50" r:id="rId48" display="Babak Momeni, Ehsan Shah Hosseini, Murtaza Askari, Mohammad Soltani, Ali Adibi, Integrated photonic crystal spectrometers for sensing applications, Optics Communications, Volume 282, Issue 15, 2009"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5454,13 +5478,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>6</v>
@@ -5469,28 +5493,28 @@
         <v>7</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>13</v>
@@ -5499,12 +5523,12 @@
         <v>14</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B3" s="27" t="n">
         <v>720</v>
@@ -5527,12 +5551,12 @@
         <v>1991</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B4" s="31" t="n">
         <v>400</v>
@@ -5563,12 +5587,12 @@
         <v>2021</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31" t="n">
@@ -5587,7 +5611,7 @@
       <c r="J5" s="32"/>
       <c r="L5" s="31"/>
       <c r="M5" s="31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>17</v>
@@ -5596,7 +5620,7 @@
         <v>2014</v>
       </c>
       <c r="P5" s="33" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
@@ -5621,7 +5645,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="31"/>
       <c r="M6" s="31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="N6" s="31" t="s">
         <v>17</v>
@@ -5630,7 +5654,7 @@
         <v>2019</v>
       </c>
       <c r="P6" s="35" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5648,13 +5672,13 @@
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I7" s="32"/>
       <c r="J7" s="32"/>
       <c r="L7" s="31"/>
       <c r="M7" s="31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="N7" s="31" t="s">
         <v>17</v>
@@ -5663,7 +5687,7 @@
         <v>2020</v>
       </c>
       <c r="P7" s="36" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
@@ -5682,7 +5706,7 @@
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
@@ -5698,12 +5722,12 @@
         <v>2011</v>
       </c>
       <c r="P8" s="35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B9" s="31" t="n">
         <v>300</v>
@@ -5717,16 +5741,16 @@
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H9" s="32" t="n">
         <v>25</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K9" s="31" t="n">
         <v>100</v>
@@ -5738,12 +5762,12 @@
         <v>2009</v>
       </c>
       <c r="P9" s="33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="30" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B10" s="31" t="n">
         <v>350</v>
@@ -5757,13 +5781,13 @@
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H10" s="32" t="n">
         <v>30</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J10" s="32" t="n">
         <v>-2</v>
@@ -5780,12 +5804,12 @@
         <v>2013</v>
       </c>
       <c r="P10" s="33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="30" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B11" s="31" t="n">
         <v>300</v>
@@ -5799,13 +5823,13 @@
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
       <c r="G11" s="31" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H11" s="32" t="n">
         <v>40</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J11" s="32" t="n">
         <v>-6</v>
@@ -5822,12 +5846,12 @@
         <v>2013</v>
       </c>
       <c r="P11" s="33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B12" s="31" t="n">
         <v>300</v>
@@ -5841,13 +5865,13 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H12" s="32" t="n">
         <v>70</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J12" s="32" t="n">
         <v>-1</v>
@@ -5864,12 +5888,12 @@
         <v>2014</v>
       </c>
       <c r="P12" s="33" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B13" s="31" t="n">
         <v>400</v>
@@ -5883,13 +5907,13 @@
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
       <c r="G13" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H13" s="32" t="n">
         <v>76</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J13" s="32" t="n">
         <v>-5</v>
@@ -5906,12 +5930,12 @@
         <v>2015</v>
       </c>
       <c r="P13" s="33" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B14" s="31" t="n">
         <v>610</v>
@@ -5927,13 +5951,13 @@
         <v>85</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H14" s="32" t="n">
         <v>35</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J14" s="32" t="n">
         <v>-1</v>
@@ -5950,12 +5974,12 @@
         <v>2015</v>
       </c>
       <c r="P14" s="33" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="30" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B15" s="31" t="n">
         <v>300</v>
@@ -5969,16 +5993,16 @@
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H15" s="32" t="n">
         <v>28</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K15" s="31" t="n">
         <v>148</v>
@@ -5992,12 +6016,12 @@
         <v>2015</v>
       </c>
       <c r="P15" s="33" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B16" s="31" t="n">
         <v>600</v>
@@ -6011,13 +6035,13 @@
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
       <c r="G16" s="31" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H16" s="32" t="n">
         <v>23</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J16" s="32" t="n">
         <v>-2</v>
@@ -6032,12 +6056,12 @@
         <v>2015</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B17" s="31" t="n">
         <v>900</v>
@@ -6053,13 +6077,13 @@
         <v>80</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J17" s="32" t="n">
         <v>-1</v>
@@ -6072,12 +6096,12 @@
         <v>2015</v>
       </c>
       <c r="P17" s="33" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B18" s="31" t="n">
         <v>300</v>
@@ -6091,13 +6115,13 @@
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="31" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H18" s="32" t="n">
         <v>27</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J18" s="32" t="n">
         <v>-2</v>
@@ -6114,12 +6138,12 @@
         <v>2016</v>
       </c>
       <c r="P18" s="33" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="30" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B19" s="31" t="n">
         <v>650</v>
@@ -6135,13 +6159,13 @@
         <v>100</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H19" s="32" t="n">
         <v>200</v>
       </c>
       <c r="I19" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J19" s="32" t="n">
         <v>-6</v>
@@ -6158,12 +6182,12 @@
         <v>2016</v>
       </c>
       <c r="P19" s="33" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B20" s="31" t="n">
         <v>640</v>
@@ -6179,7 +6203,7 @@
         <v>28</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H20" s="32" t="n">
         <v>53500</v>
@@ -6200,12 +6224,12 @@
         <v>2017</v>
       </c>
       <c r="P20" s="33" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B21" s="31" t="n">
         <v>700</v>
@@ -6221,13 +6245,13 @@
         <v>15</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H21" s="32" t="n">
         <v>40</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J21" s="32" t="n">
         <v>0</v>
@@ -6242,12 +6266,12 @@
         <v>2017</v>
       </c>
       <c r="P21" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B22" s="31" t="n">
         <v>700</v>
@@ -6263,13 +6287,13 @@
         <v>17</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H22" s="32" t="n">
         <v>24</v>
       </c>
       <c r="I22" s="32" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J22" s="32" t="n">
         <v>0</v>
@@ -6284,12 +6308,12 @@
         <v>2017</v>
       </c>
       <c r="P22" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B23" s="31" t="n">
         <v>1000</v>
@@ -6305,13 +6329,13 @@
         <v>35</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J23" s="32" t="n">
         <v>0</v>
@@ -6324,12 +6348,12 @@
         <v>2017</v>
       </c>
       <c r="P23" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B24" s="31" t="n">
         <v>1000</v>
@@ -6345,13 +6369,13 @@
         <v>38</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J24" s="32" t="n">
         <v>0</v>
@@ -6364,12 +6388,12 @@
         <v>2017</v>
       </c>
       <c r="P24" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B25" s="31" t="n">
         <v>1000</v>
@@ -6385,13 +6409,13 @@
         <v>47</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J25" s="32" t="n">
         <v>0</v>
@@ -6404,12 +6428,12 @@
         <v>2017</v>
       </c>
       <c r="P25" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B26" s="31" t="n">
         <v>1000</v>
@@ -6425,13 +6449,13 @@
         <v>41</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H26" s="32" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I26" s="32" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="J26" s="32" t="n">
         <v>0</v>
@@ -6444,12 +6468,12 @@
         <v>2017</v>
       </c>
       <c r="P26" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B27" s="31" t="n">
         <v>875</v>
@@ -6465,13 +6489,13 @@
         <v>43</v>
       </c>
       <c r="G27" s="31" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H27" s="32" t="n">
         <v>22</v>
       </c>
       <c r="I27" s="32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J27" s="32" t="n">
         <v>0</v>
@@ -6486,12 +6510,12 @@
         <v>2017</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B28" s="31" t="n">
         <v>810</v>
@@ -6516,12 +6540,12 @@
         <v>2017</v>
       </c>
       <c r="P28" s="33" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="30" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B29" s="31" t="n">
         <v>400</v>
@@ -6535,13 +6559,13 @@
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J29" s="32" t="n">
         <v>-40</v>
@@ -6556,12 +6580,12 @@
         <v>2018</v>
       </c>
       <c r="P29" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="30" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B30" s="31" t="n">
         <v>300</v>
@@ -6575,13 +6599,13 @@
       <c r="E30" s="31"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H30" s="32" t="n">
         <v>48</v>
       </c>
       <c r="I30" s="32" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J30" s="32" t="n">
         <v>0</v>
@@ -6594,12 +6618,12 @@
         <v>2018</v>
       </c>
       <c r="P30" s="33" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B31" s="31" t="n">
         <v>790</v>
@@ -6615,13 +6639,13 @@
         <v>30</v>
       </c>
       <c r="G31" s="31" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H31" s="32" t="n">
         <v>2000</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="J31" s="32" t="n">
         <v>-50</v>
@@ -6636,12 +6660,12 @@
         <v>2018</v>
       </c>
       <c r="P31" s="33" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="30" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B32" s="31" t="n">
         <v>350</v>
@@ -6657,20 +6681,20 @@
         <v>20</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H32" s="32" t="n">
         <v>2170</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="J32" s="32" t="n">
         <v>-15</v>
       </c>
       <c r="K32" s="31"/>
       <c r="L32" s="31" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M32" s="31"/>
       <c r="N32" s="31"/>
@@ -6678,12 +6702,12 @@
         <v>2018</v>
       </c>
       <c r="P32" s="33" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="30" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B33" s="31" t="n">
         <v>300</v>
@@ -6697,16 +6721,16 @@
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H33" s="32" t="n">
         <v>56</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K33" s="31" t="n">
         <v>97</v>
@@ -6720,12 +6744,12 @@
         <v>2019</v>
       </c>
       <c r="P33" s="33" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="30" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B34" s="31" t="n">
         <v>420</v>
@@ -6741,13 +6765,13 @@
         <v>76</v>
       </c>
       <c r="G34" s="31" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H34" s="32" t="n">
         <v>18</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J34" s="32" t="n">
         <v>0</v>
@@ -6760,12 +6784,12 @@
         <v>2019</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B35" s="31" t="n">
         <v>400</v>
@@ -6781,13 +6805,13 @@
         <v>84</v>
       </c>
       <c r="G35" s="31" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H35" s="32" t="n">
         <v>50</v>
       </c>
       <c r="I35" s="32" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J35" s="32" t="n">
         <v>0</v>
@@ -6804,12 +6828,12 @@
         <v>2019</v>
       </c>
       <c r="P35" s="33" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B36" s="31" t="n">
         <v>810</v>
@@ -6825,13 +6849,13 @@
         <v>50</v>
       </c>
       <c r="G36" s="31" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I36" s="32" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J36" s="32" t="n">
         <v>0</v>
@@ -6844,12 +6868,12 @@
         <v>2019</v>
       </c>
       <c r="P36" s="37" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="30" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B37" s="31" t="n">
         <v>810</v>
@@ -6865,13 +6889,13 @@
         <v>50</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="J37" s="32" t="n">
         <v>0</v>
@@ -6884,12 +6908,12 @@
         <v>2019</v>
       </c>
       <c r="P37" s="37" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="30" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B38" s="31" t="n">
         <v>300</v>
@@ -6903,13 +6927,13 @@
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
       <c r="G38" s="31" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I38" s="32" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="J38" s="32" t="n">
         <v>-2</v>
@@ -6918,7 +6942,7 @@
         <v>173</v>
       </c>
       <c r="L38" s="31" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="M38" s="31"/>
       <c r="N38" s="31"/>
@@ -6926,12 +6950,12 @@
         <v>2020</v>
       </c>
       <c r="P38" s="33" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="30" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B39" s="31" t="n">
         <v>645</v>
@@ -6947,13 +6971,13 @@
         <v>50</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I39" s="32" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="J39" s="32" t="n">
         <v>0</v>
@@ -6962,7 +6986,7 @@
         <v>103</v>
       </c>
       <c r="L39" s="31" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="M39" s="31"/>
       <c r="N39" s="31"/>
@@ -6970,12 +6994,12 @@
         <v>2020</v>
       </c>
       <c r="P39" s="33" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="30" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B40" s="31" t="n">
         <v>860</v>
@@ -6991,16 +7015,16 @@
         <v>50</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H40" s="32" t="n">
         <v>61</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="J40" s="32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K40" s="31"/>
       <c r="L40" s="31"/>
@@ -7010,12 +7034,12 @@
         <v>2020</v>
       </c>
       <c r="P40" s="33" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="30" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B41" s="31" t="n">
         <v>860</v>
@@ -7031,12 +7055,12 @@
         <v>40</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
       <c r="J41" s="32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K41" s="31"/>
       <c r="L41" s="31"/>
@@ -7046,12 +7070,12 @@
         <v>2020</v>
       </c>
       <c r="P41" s="33" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="30" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B42" s="31" t="n">
         <v>860</v>
@@ -7067,12 +7091,12 @@
         <v>50</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
       <c r="J42" s="32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K42" s="31"/>
       <c r="L42" s="31"/>
@@ -7082,12 +7106,12 @@
         <v>2020</v>
       </c>
       <c r="P42" s="33" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="30" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B43" s="31" t="n">
         <v>750</v>
@@ -7103,13 +7127,13 @@
         <v>120</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H43" s="32" t="n">
         <v>53</v>
       </c>
       <c r="I43" s="32" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J43" s="32" t="n">
         <v>0</v>
@@ -7124,12 +7148,12 @@
         <v>2020</v>
       </c>
       <c r="P43" s="33" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B44" s="31" t="n">
         <v>790</v>
@@ -7145,13 +7169,13 @@
         <v>37</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H44" s="32" t="n">
         <v>10</v>
       </c>
       <c r="I44" s="32" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="J44" s="32" t="n">
         <v>0</v>
@@ -7166,12 +7190,12 @@
         <v>2020</v>
       </c>
       <c r="P44" s="33" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="30" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B45" s="31" t="n">
         <v>1020</v>
@@ -7187,13 +7211,13 @@
         <v>58</v>
       </c>
       <c r="G45" s="31" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H45" s="32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I45" s="32" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="J45" s="32" t="n">
         <v>0</v>
@@ -7208,12 +7232,12 @@
         <v>2020</v>
       </c>
       <c r="P45" s="33" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="30" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B46" s="31" t="n">
         <v>300</v>
@@ -7227,16 +7251,16 @@
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
       <c r="G46" s="31" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="J46" s="32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K46" s="31" t="n">
         <v>123</v>
@@ -7250,12 +7274,12 @@
         <v>2021</v>
       </c>
       <c r="P46" s="33" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="30" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B47" s="31" t="n">
         <v>830</v>
@@ -7271,7 +7295,7 @@
         <v>27</v>
       </c>
       <c r="G47" s="31" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="H47" s="32" t="n">
         <v>15300</v>
@@ -7292,12 +7316,12 @@
         <v>2021</v>
       </c>
       <c r="P47" s="33" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="30" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B48" s="31" t="n">
         <v>650</v>
@@ -7313,13 +7337,13 @@
         <v>60</v>
       </c>
       <c r="G48" s="31" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H48" s="32" t="n">
         <v>18</v>
       </c>
       <c r="I48" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J48" s="32" t="n">
         <v>0</v>
@@ -7334,12 +7358,12 @@
         <v>2021</v>
       </c>
       <c r="P48" s="33" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="30" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B49" s="31" t="n">
         <v>650</v>
@@ -7355,13 +7379,13 @@
         <v>45</v>
       </c>
       <c r="G49" s="31" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H49" s="32" t="n">
         <v>6</v>
       </c>
       <c r="I49" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J49" s="32" t="n">
         <v>0</v>
@@ -7374,12 +7398,12 @@
         <v>2021</v>
       </c>
       <c r="P49" s="33" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="30" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B50" s="31" t="n">
         <v>650</v>
@@ -7395,13 +7419,13 @@
         <v>35</v>
       </c>
       <c r="G50" s="31" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="H50" s="32" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="J50" s="32" t="n">
         <v>0</v>
@@ -7414,12 +7438,12 @@
         <v>2021</v>
       </c>
       <c r="P50" s="33" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="30" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B51" s="31" t="n">
         <v>650</v>
@@ -7435,13 +7459,13 @@
         <v>20</v>
       </c>
       <c r="G51" s="31" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="H51" s="32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I51" s="32" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="J51" s="32" t="n">
         <v>0</v>
@@ -7454,12 +7478,12 @@
         <v>2021</v>
       </c>
       <c r="P51" s="33" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B52" s="31" t="n">
         <v>826</v>
@@ -7475,20 +7499,20 @@
         <v>17</v>
       </c>
       <c r="G52" s="31" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H52" s="32" t="n">
         <v>75</v>
       </c>
       <c r="I52" s="32" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="J52" s="32" t="n">
         <v>-10</v>
       </c>
       <c r="K52" s="31"/>
       <c r="L52" s="31" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M52" s="31"/>
       <c r="N52" s="31"/>
@@ -7496,7 +7520,7 @@
         <v>2021</v>
       </c>
       <c r="P52" s="33" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7931,13 +7955,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="39" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7987,13 +8011,13 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38"/>
       <c r="B8" s="38" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38"/>
       <c r="B9" s="40" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8011,7 +8035,7 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38"/>
       <c r="B12" s="38" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8023,7 +8047,7 @@
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38"/>
       <c r="B14" s="38" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8035,277 +8059,277 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38"/>
       <c r="B16" s="38" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38"/>
       <c r="B17" s="38" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38"/>
       <c r="B18" s="38" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38"/>
       <c r="B19" s="38" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38"/>
       <c r="B20" s="38" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38"/>
       <c r="B21" s="38" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38"/>
       <c r="B22" s="38" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38"/>
       <c r="B23" s="38" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38"/>
       <c r="B24" s="38" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38"/>
       <c r="B25" s="38" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="38"/>
       <c r="B26" s="38" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38"/>
       <c r="B27" s="38" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38"/>
       <c r="B28" s="38" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38"/>
       <c r="B29" s="38" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38"/>
       <c r="B30" s="38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="38"/>
       <c r="B31" s="38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="38"/>
       <c r="B32" s="38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="38"/>
       <c r="B33" s="38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="38"/>
       <c r="B34" s="38" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="38"/>
       <c r="B35" s="38" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="38"/>
       <c r="B36" s="38" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="38"/>
       <c r="B37" s="38" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="38"/>
       <c r="B38" s="38" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="38"/>
       <c r="B39" s="38" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="38"/>
       <c r="B40" s="38" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="38"/>
       <c r="B41" s="38" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="38"/>
       <c r="B42" s="38" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="38"/>
       <c r="B43" s="38" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="38"/>
       <c r="B44" s="38" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="38"/>
       <c r="B45" s="38" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="38"/>
       <c r="B46" s="38" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="38"/>
       <c r="B47" s="38" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="38"/>
       <c r="B48" s="38" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="38"/>
       <c r="B49" s="38" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="38"/>
       <c r="B50" s="38" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="38"/>
       <c r="B51" s="38" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="38"/>
       <c r="B52" s="38" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="38"/>
       <c r="B53" s="38" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="38"/>
       <c r="B54" s="38" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="38"/>
       <c r="B55" s="38" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="38"/>
       <c r="B56" s="38" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="38"/>
       <c r="B57" s="38" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="38"/>
       <c r="B58" s="38" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="38"/>
       <c r="B59" s="38" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="38"/>
       <c r="B60" s="38" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="38"/>
       <c r="B61" s="41" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add refs ma2018 and zhang2024
</commit_message>
<xml_diff>
--- a/iPHAOS.xlsx
+++ b/iPHAOS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="279">
   <si>
     <t xml:space="preserve">Spectral range</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t xml:space="preserve">Babak Momeni, Ehsan Shah Hosseini, Murtaza Askari, Mohammad Soltani, Ali Adibi, Integrated photonic crystal spectrometers for sensing applications, Optics Communications, Volume 282, Issue 15, 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 x 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K. Ma, K. Chen, N. Zhu, L. Liu and S. He, "High-Resolution Compact On-Chip Spectrometer Based on an Echelle Grating With Densely Packed Waveguide Array," in IEEE Photonics Journal, vol. 11, no. 1, pp. 1-7, Feb. 2019, Art no. 4900107, doi: 10.1109/JPHOT.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhang, Z.; Huang, B.; Zhang, Z.; Chen, H. On-Chip Reconstructive Spectrometer Based on Parallel Cascaded Micro-Ring Resonators. Appl. Sci. 2024, 14, 4886. https://doi.org/10.3390/app14114886</t>
   </si>
   <si>
     <t xml:space="preserve">Material</t>
@@ -1465,8 +1474,8 @@
   </sheetPr>
   <dimension ref="A1:O268"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O13" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O50" activeCellId="0" sqref="O50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O28" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O51" activeCellId="0" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3389,44 +3398,78 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
+      <c r="A51" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
+      <c r="G51" s="14" t="n">
+        <v>0.5</v>
+      </c>
       <c r="H51" s="15" t="str">
         <f aca="false">IF(AND(E51&lt;&gt;0,G51&lt;&gt;0),E51/G51,"")</f>
         <v/>
       </c>
       <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
+      <c r="J51" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="K51" s="14"/>
       <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="19"/>
+      <c r="M51" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N51" s="14" t="n">
+        <v>2018</v>
+      </c>
+      <c r="O51" s="19" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="15" t="str">
+      <c r="A52" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="14" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D52" s="14" t="n">
+        <v>1650</v>
+      </c>
+      <c r="E52" s="14" t="n">
+        <v>200</v>
+      </c>
+      <c r="F52" s="14" t="n">
+        <v>1550</v>
+      </c>
+      <c r="G52" s="14" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H52" s="15" t="n">
         <f aca="false">IF(AND(E52&lt;&gt;0,G52&lt;&gt;0),E52/G52,"")</f>
-        <v/>
+        <v>20000</v>
       </c>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
       <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="19"/>
+      <c r="M52" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N52" s="14" t="n">
+        <v>2024</v>
+      </c>
+      <c r="O52" s="19" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="14"/>
@@ -5428,6 +5471,8 @@
     <hyperlink ref="O48" r:id="rId46" display="J. Brouckaert, W. Bogaerts, S. Selvaraja, P. Dumon, R. Baets and D. Van Thourhout, &quot;Planar Concave Grating Demultiplexer With High Reflective Bragg Reflector Facets,&quot; in IEEE Photonics Technology Letters, vol. 20, no. 4, pp. 309-311, Feb.15, 2008, doi: 10"/>
     <hyperlink ref="O49" r:id="rId47" location="citeas" display="Redding, B., Liew, S., Sarma, R. et al. Compact spectrometer based on a disordered photonic chip. Nature Photon 7, 746–751 (2013). https://doi.org/10.1038/nphoton.2013.190"/>
     <hyperlink ref="O50" r:id="rId48" display="Babak Momeni, Ehsan Shah Hosseini, Murtaza Askari, Mohammad Soltani, Ali Adibi, Integrated photonic crystal spectrometers for sensing applications, Optics Communications, Volume 282, Issue 15, 2009"/>
+    <hyperlink ref="O51" r:id="rId49" display="K. Ma, K. Chen, N. Zhu, L. Liu and S. He, &quot;High-Resolution Compact On-Chip Spectrometer Based on an Echelle Grating With Densely Packed Waveguide Array,&quot; in IEEE Photonics Journal, vol. 11, no. 1, pp. 1-7, Feb. 2019, Art no. 4900107, doi: 10.1109/JPHOT.20"/>
+    <hyperlink ref="O52" r:id="rId50" display="Zhang, Z.; Huang, B.; Zhang, Z.; Chen, H. On-Chip Reconstructive Spectrometer Based on Parallel Cascaded Micro-Ring Resonators. Appl. Sci. 2024, 14, 4886. https://doi.org/10.3390/app14114886"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5450,7 +5495,7 @@
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.86"/>
@@ -5478,13 +5523,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>6</v>
@@ -5493,28 +5538,28 @@
         <v>7</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>13</v>
@@ -5523,12 +5568,12 @@
         <v>14</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B3" s="27" t="n">
         <v>720</v>
@@ -5551,12 +5596,12 @@
         <v>1991</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B4" s="31" t="n">
         <v>400</v>
@@ -5587,12 +5632,12 @@
         <v>2021</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31" t="n">
@@ -5611,7 +5656,7 @@
       <c r="J5" s="32"/>
       <c r="L5" s="31"/>
       <c r="M5" s="31" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>17</v>
@@ -5620,7 +5665,7 @@
         <v>2014</v>
       </c>
       <c r="P5" s="33" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
@@ -5645,7 +5690,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="31"/>
       <c r="M6" s="31" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="N6" s="31" t="s">
         <v>17</v>
@@ -5654,7 +5699,7 @@
         <v>2019</v>
       </c>
       <c r="P6" s="35" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5672,13 +5717,13 @@
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="32" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I7" s="32"/>
       <c r="J7" s="32"/>
       <c r="L7" s="31"/>
       <c r="M7" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="N7" s="31" t="s">
         <v>17</v>
@@ -5687,7 +5732,7 @@
         <v>2020</v>
       </c>
       <c r="P7" s="36" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
@@ -5706,7 +5751,7 @@
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="32" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
@@ -5722,12 +5767,12 @@
         <v>2011</v>
       </c>
       <c r="P8" s="35" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B9" s="31" t="n">
         <v>300</v>
@@ -5741,16 +5786,16 @@
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H9" s="32" t="n">
         <v>25</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K9" s="31" t="n">
         <v>100</v>
@@ -5762,12 +5807,12 @@
         <v>2009</v>
       </c>
       <c r="P9" s="33" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="30" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B10" s="31" t="n">
         <v>350</v>
@@ -5781,13 +5826,13 @@
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H10" s="32" t="n">
         <v>30</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J10" s="32" t="n">
         <v>-2</v>
@@ -5804,12 +5849,12 @@
         <v>2013</v>
       </c>
       <c r="P10" s="33" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="30" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B11" s="31" t="n">
         <v>300</v>
@@ -5823,13 +5868,13 @@
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
       <c r="G11" s="31" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H11" s="32" t="n">
         <v>40</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J11" s="32" t="n">
         <v>-6</v>
@@ -5846,12 +5891,12 @@
         <v>2013</v>
       </c>
       <c r="P11" s="33" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B12" s="31" t="n">
         <v>300</v>
@@ -5865,13 +5910,13 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H12" s="32" t="n">
         <v>70</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="J12" s="32" t="n">
         <v>-1</v>
@@ -5888,12 +5933,12 @@
         <v>2014</v>
       </c>
       <c r="P12" s="33" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="30" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B13" s="31" t="n">
         <v>400</v>
@@ -5907,13 +5952,13 @@
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
       <c r="G13" s="31" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H13" s="32" t="n">
         <v>76</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J13" s="32" t="n">
         <v>-5</v>
@@ -5930,12 +5975,12 @@
         <v>2015</v>
       </c>
       <c r="P13" s="33" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B14" s="31" t="n">
         <v>610</v>
@@ -5951,13 +5996,13 @@
         <v>85</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H14" s="32" t="n">
         <v>35</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J14" s="32" t="n">
         <v>-1</v>
@@ -5974,12 +6019,12 @@
         <v>2015</v>
       </c>
       <c r="P14" s="33" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="30" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B15" s="31" t="n">
         <v>300</v>
@@ -5993,16 +6038,16 @@
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H15" s="32" t="n">
         <v>28</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K15" s="31" t="n">
         <v>148</v>
@@ -6016,12 +6061,12 @@
         <v>2015</v>
       </c>
       <c r="P15" s="33" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="30" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B16" s="31" t="n">
         <v>600</v>
@@ -6035,13 +6080,13 @@
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
       <c r="G16" s="31" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H16" s="32" t="n">
         <v>23</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J16" s="32" t="n">
         <v>-2</v>
@@ -6056,12 +6101,12 @@
         <v>2015</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B17" s="31" t="n">
         <v>900</v>
@@ -6077,13 +6122,13 @@
         <v>80</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J17" s="32" t="n">
         <v>-1</v>
@@ -6096,12 +6141,12 @@
         <v>2015</v>
       </c>
       <c r="P17" s="33" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B18" s="31" t="n">
         <v>300</v>
@@ -6115,13 +6160,13 @@
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="31" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H18" s="32" t="n">
         <v>27</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J18" s="32" t="n">
         <v>-2</v>
@@ -6138,12 +6183,12 @@
         <v>2016</v>
       </c>
       <c r="P18" s="33" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="30" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B19" s="31" t="n">
         <v>650</v>
@@ -6159,13 +6204,13 @@
         <v>100</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H19" s="32" t="n">
         <v>200</v>
       </c>
       <c r="I19" s="32" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="J19" s="32" t="n">
         <v>-6</v>
@@ -6182,12 +6227,12 @@
         <v>2016</v>
       </c>
       <c r="P19" s="33" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B20" s="31" t="n">
         <v>640</v>
@@ -6203,7 +6248,7 @@
         <v>28</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H20" s="32" t="n">
         <v>53500</v>
@@ -6224,12 +6269,12 @@
         <v>2017</v>
       </c>
       <c r="P20" s="33" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B21" s="31" t="n">
         <v>700</v>
@@ -6245,13 +6290,13 @@
         <v>15</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H21" s="32" t="n">
         <v>40</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="J21" s="32" t="n">
         <v>0</v>
@@ -6266,12 +6311,12 @@
         <v>2017</v>
       </c>
       <c r="P21" s="33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B22" s="31" t="n">
         <v>700</v>
@@ -6287,13 +6332,13 @@
         <v>17</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H22" s="32" t="n">
         <v>24</v>
       </c>
       <c r="I22" s="32" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J22" s="32" t="n">
         <v>0</v>
@@ -6308,12 +6353,12 @@
         <v>2017</v>
       </c>
       <c r="P22" s="33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B23" s="31" t="n">
         <v>1000</v>
@@ -6329,13 +6374,13 @@
         <v>35</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="J23" s="32" t="n">
         <v>0</v>
@@ -6348,12 +6393,12 @@
         <v>2017</v>
       </c>
       <c r="P23" s="33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="30" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B24" s="31" t="n">
         <v>1000</v>
@@ -6369,13 +6414,13 @@
         <v>38</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J24" s="32" t="n">
         <v>0</v>
@@ -6388,12 +6433,12 @@
         <v>2017</v>
       </c>
       <c r="P24" s="33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B25" s="31" t="n">
         <v>1000</v>
@@ -6409,13 +6454,13 @@
         <v>47</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J25" s="32" t="n">
         <v>0</v>
@@ -6428,12 +6473,12 @@
         <v>2017</v>
       </c>
       <c r="P25" s="33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B26" s="31" t="n">
         <v>1000</v>
@@ -6449,13 +6494,13 @@
         <v>41</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H26" s="32" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="I26" s="32" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="J26" s="32" t="n">
         <v>0</v>
@@ -6468,12 +6513,12 @@
         <v>2017</v>
       </c>
       <c r="P26" s="33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="30" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B27" s="31" t="n">
         <v>875</v>
@@ -6489,13 +6534,13 @@
         <v>43</v>
       </c>
       <c r="G27" s="31" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H27" s="32" t="n">
         <v>22</v>
       </c>
       <c r="I27" s="32" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J27" s="32" t="n">
         <v>0</v>
@@ -6510,12 +6555,12 @@
         <v>2017</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="30" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B28" s="31" t="n">
         <v>810</v>
@@ -6540,12 +6585,12 @@
         <v>2017</v>
       </c>
       <c r="P28" s="33" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="30" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B29" s="31" t="n">
         <v>400</v>
@@ -6559,13 +6604,13 @@
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J29" s="32" t="n">
         <v>-40</v>
@@ -6580,12 +6625,12 @@
         <v>2018</v>
       </c>
       <c r="P29" s="33" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="30" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B30" s="31" t="n">
         <v>300</v>
@@ -6599,13 +6644,13 @@
       <c r="E30" s="31"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H30" s="32" t="n">
         <v>48</v>
       </c>
       <c r="I30" s="32" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J30" s="32" t="n">
         <v>0</v>
@@ -6618,12 +6663,12 @@
         <v>2018</v>
       </c>
       <c r="P30" s="33" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B31" s="31" t="n">
         <v>790</v>
@@ -6639,13 +6684,13 @@
         <v>30</v>
       </c>
       <c r="G31" s="31" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H31" s="32" t="n">
         <v>2000</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J31" s="32" t="n">
         <v>-50</v>
@@ -6660,12 +6705,12 @@
         <v>2018</v>
       </c>
       <c r="P31" s="33" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="30" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B32" s="31" t="n">
         <v>350</v>
@@ -6681,20 +6726,20 @@
         <v>20</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H32" s="32" t="n">
         <v>2170</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="J32" s="32" t="n">
         <v>-15</v>
       </c>
       <c r="K32" s="31"/>
       <c r="L32" s="31" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="M32" s="31"/>
       <c r="N32" s="31"/>
@@ -6702,12 +6747,12 @@
         <v>2018</v>
       </c>
       <c r="P32" s="33" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="30" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B33" s="31" t="n">
         <v>300</v>
@@ -6721,16 +6766,16 @@
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H33" s="32" t="n">
         <v>56</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K33" s="31" t="n">
         <v>97</v>
@@ -6744,12 +6789,12 @@
         <v>2019</v>
       </c>
       <c r="P33" s="33" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="30" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B34" s="31" t="n">
         <v>420</v>
@@ -6765,13 +6810,13 @@
         <v>76</v>
       </c>
       <c r="G34" s="31" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="H34" s="32" t="n">
         <v>18</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="J34" s="32" t="n">
         <v>0</v>
@@ -6784,12 +6829,12 @@
         <v>2019</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B35" s="31" t="n">
         <v>400</v>
@@ -6805,13 +6850,13 @@
         <v>84</v>
       </c>
       <c r="G35" s="31" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H35" s="32" t="n">
         <v>50</v>
       </c>
       <c r="I35" s="32" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="J35" s="32" t="n">
         <v>0</v>
@@ -6828,12 +6873,12 @@
         <v>2019</v>
       </c>
       <c r="P35" s="33" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B36" s="31" t="n">
         <v>810</v>
@@ -6849,13 +6894,13 @@
         <v>50</v>
       </c>
       <c r="G36" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I36" s="32" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="J36" s="32" t="n">
         <v>0</v>
@@ -6868,12 +6913,12 @@
         <v>2019</v>
       </c>
       <c r="P36" s="37" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="30" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B37" s="31" t="n">
         <v>810</v>
@@ -6889,13 +6934,13 @@
         <v>50</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J37" s="32" t="n">
         <v>0</v>
@@ -6908,12 +6953,12 @@
         <v>2019</v>
       </c>
       <c r="P37" s="37" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B38" s="31" t="n">
         <v>300</v>
@@ -6927,13 +6972,13 @@
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
       <c r="G38" s="31" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="I38" s="32" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J38" s="32" t="n">
         <v>-2</v>
@@ -6942,7 +6987,7 @@
         <v>173</v>
       </c>
       <c r="L38" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="M38" s="31"/>
       <c r="N38" s="31"/>
@@ -6950,12 +6995,12 @@
         <v>2020</v>
       </c>
       <c r="P38" s="33" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="30" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B39" s="31" t="n">
         <v>645</v>
@@ -6971,13 +7016,13 @@
         <v>50</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="I39" s="32" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J39" s="32" t="n">
         <v>0</v>
@@ -6986,7 +7031,7 @@
         <v>103</v>
       </c>
       <c r="L39" s="31" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="M39" s="31"/>
       <c r="N39" s="31"/>
@@ -6994,12 +7039,12 @@
         <v>2020</v>
       </c>
       <c r="P39" s="33" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="30" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B40" s="31" t="n">
         <v>860</v>
@@ -7015,16 +7060,16 @@
         <v>50</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="H40" s="32" t="n">
         <v>61</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J40" s="32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K40" s="31"/>
       <c r="L40" s="31"/>
@@ -7034,12 +7079,12 @@
         <v>2020</v>
       </c>
       <c r="P40" s="33" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="30" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B41" s="31" t="n">
         <v>860</v>
@@ -7055,12 +7100,12 @@
         <v>40</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
       <c r="J41" s="32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K41" s="31"/>
       <c r="L41" s="31"/>
@@ -7070,12 +7115,12 @@
         <v>2020</v>
       </c>
       <c r="P41" s="33" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="30" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B42" s="31" t="n">
         <v>860</v>
@@ -7091,12 +7136,12 @@
         <v>50</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
       <c r="J42" s="32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K42" s="31"/>
       <c r="L42" s="31"/>
@@ -7106,12 +7151,12 @@
         <v>2020</v>
       </c>
       <c r="P42" s="33" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B43" s="31" t="n">
         <v>750</v>
@@ -7127,13 +7172,13 @@
         <v>120</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H43" s="32" t="n">
         <v>53</v>
       </c>
       <c r="I43" s="32" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="J43" s="32" t="n">
         <v>0</v>
@@ -7148,12 +7193,12 @@
         <v>2020</v>
       </c>
       <c r="P43" s="33" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="30" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B44" s="31" t="n">
         <v>790</v>
@@ -7169,13 +7214,13 @@
         <v>37</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H44" s="32" t="n">
         <v>10</v>
       </c>
       <c r="I44" s="32" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J44" s="32" t="n">
         <v>0</v>
@@ -7190,12 +7235,12 @@
         <v>2020</v>
       </c>
       <c r="P44" s="33" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="30" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B45" s="31" t="n">
         <v>1020</v>
@@ -7211,13 +7256,13 @@
         <v>58</v>
       </c>
       <c r="G45" s="31" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H45" s="32" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I45" s="32" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="J45" s="32" t="n">
         <v>0</v>
@@ -7232,12 +7277,12 @@
         <v>2020</v>
       </c>
       <c r="P45" s="33" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="30" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B46" s="31" t="n">
         <v>300</v>
@@ -7251,16 +7296,16 @@
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
       <c r="G46" s="31" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="J46" s="32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K46" s="31" t="n">
         <v>123</v>
@@ -7274,12 +7319,12 @@
         <v>2021</v>
       </c>
       <c r="P46" s="33" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="30" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B47" s="31" t="n">
         <v>830</v>
@@ -7295,7 +7340,7 @@
         <v>27</v>
       </c>
       <c r="G47" s="31" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="H47" s="32" t="n">
         <v>15300</v>
@@ -7316,12 +7361,12 @@
         <v>2021</v>
       </c>
       <c r="P47" s="33" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="30" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B48" s="31" t="n">
         <v>650</v>
@@ -7337,13 +7382,13 @@
         <v>60</v>
       </c>
       <c r="G48" s="31" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="H48" s="32" t="n">
         <v>18</v>
       </c>
       <c r="I48" s="32" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J48" s="32" t="n">
         <v>0</v>
@@ -7358,12 +7403,12 @@
         <v>2021</v>
       </c>
       <c r="P48" s="33" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="30" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B49" s="31" t="n">
         <v>650</v>
@@ -7379,13 +7424,13 @@
         <v>45</v>
       </c>
       <c r="G49" s="31" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H49" s="32" t="n">
         <v>6</v>
       </c>
       <c r="I49" s="32" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="J49" s="32" t="n">
         <v>0</v>
@@ -7398,12 +7443,12 @@
         <v>2021</v>
       </c>
       <c r="P49" s="33" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="30" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B50" s="31" t="n">
         <v>650</v>
@@ -7419,13 +7464,13 @@
         <v>35</v>
       </c>
       <c r="G50" s="31" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H50" s="32" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="J50" s="32" t="n">
         <v>0</v>
@@ -7438,12 +7483,12 @@
         <v>2021</v>
       </c>
       <c r="P50" s="33" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="30" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B51" s="31" t="n">
         <v>650</v>
@@ -7459,13 +7504,13 @@
         <v>20</v>
       </c>
       <c r="G51" s="31" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="H51" s="32" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I51" s="32" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="J51" s="32" t="n">
         <v>0</v>
@@ -7478,12 +7523,12 @@
         <v>2021</v>
       </c>
       <c r="P51" s="33" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="30" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B52" s="31" t="n">
         <v>826</v>
@@ -7499,20 +7544,20 @@
         <v>17</v>
       </c>
       <c r="G52" s="31" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="H52" s="32" t="n">
         <v>75</v>
       </c>
       <c r="I52" s="32" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="J52" s="32" t="n">
         <v>-10</v>
       </c>
       <c r="K52" s="31"/>
       <c r="L52" s="31" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="M52" s="31"/>
       <c r="N52" s="31"/>
@@ -7520,7 +7565,7 @@
         <v>2021</v>
       </c>
       <c r="P52" s="33" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7946,7 +7991,7 @@
       <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.14"/>
@@ -7955,13 +8000,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="39" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8011,13 +8056,13 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38"/>
       <c r="B8" s="38" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38"/>
       <c r="B9" s="40" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8035,7 +8080,7 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38"/>
       <c r="B12" s="38" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8047,7 +8092,7 @@
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38"/>
       <c r="B14" s="38" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8059,277 +8104,277 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38"/>
       <c r="B16" s="38" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38"/>
       <c r="B17" s="38" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38"/>
       <c r="B18" s="38" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38"/>
       <c r="B19" s="38" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38"/>
       <c r="B20" s="38" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38"/>
       <c r="B21" s="38" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38"/>
       <c r="B22" s="38" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38"/>
       <c r="B23" s="38" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38"/>
       <c r="B24" s="38" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38"/>
       <c r="B25" s="38" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="38"/>
       <c r="B26" s="38" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38"/>
       <c r="B27" s="38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38"/>
       <c r="B28" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38"/>
       <c r="B29" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38"/>
       <c r="B30" s="38" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="38"/>
       <c r="B31" s="38" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="38"/>
       <c r="B32" s="38" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="38"/>
       <c r="B33" s="38" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="38"/>
       <c r="B34" s="38" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="38"/>
       <c r="B35" s="38" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="38"/>
       <c r="B36" s="38" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="38"/>
       <c r="B37" s="38" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="38"/>
       <c r="B38" s="38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="38"/>
       <c r="B39" s="38" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="38"/>
       <c r="B40" s="38" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="38"/>
       <c r="B41" s="38" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="38"/>
       <c r="B42" s="38" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="38"/>
       <c r="B43" s="38" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="38"/>
       <c r="B44" s="38" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="38"/>
       <c r="B45" s="38" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="38"/>
       <c r="B46" s="38" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="38"/>
       <c r="B47" s="38" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="38"/>
       <c r="B48" s="38" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="38"/>
       <c r="B49" s="38" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="38"/>
       <c r="B50" s="38" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="38"/>
       <c r="B51" s="38" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="38"/>
       <c r="B52" s="38" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="38"/>
       <c r="B53" s="38" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="38"/>
       <c r="B54" s="38" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="38"/>
       <c r="B55" s="38" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="38"/>
       <c r="B56" s="38" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="38"/>
       <c r="B57" s="38" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="38"/>
       <c r="B58" s="38" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="38"/>
       <c r="B59" s="38" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="38"/>
       <c r="B60" s="38" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="38"/>
       <c r="B61" s="41" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add yao et al. 2024 Chip-scale sensor for spectroscopic metrology
</commit_message>
<xml_diff>
--- a/iPHAOS.xlsx
+++ b/iPHAOS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="285">
   <si>
     <t xml:space="preserve">Spectral range</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tian, M., Liu, B., Lu, Z. et al. Miniaturized on-chip spectrometer enabled by electrochromic modulation. Light Sci Appl 13, 278 (2024). https://doi.org/10.1038/s41377-024-01638-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 x (80e-6 × 150e-6+200e-6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yao, C., Zhang, W., Bao, P. et al. Chip-scale sensor for spectroscopic metrology. Nat Commun 15, 10305 (2024). https://doi.org/10.1038/s41467-024-54708-x</t>
   </si>
   <si>
     <t xml:space="preserve">Material</t>
@@ -999,12 +1005,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1072,12 +1079,6 @@
       <name val="Times new roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1332,55 +1333,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1388,31 +1389,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1496,8 +1497,8 @@
   </sheetPr>
   <dimension ref="A1:O268"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O28" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O54" activeCellId="0" sqref="O54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O13" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O57" activeCellId="0" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1509,7 +1510,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="28.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.92"/>
@@ -3577,23 +3578,42 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
+      <c r="B55" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="14" t="n">
+        <v>1180</v>
+      </c>
+      <c r="D55" s="14" t="n">
+        <v>1700</v>
+      </c>
+      <c r="E55" s="14" t="n">
+        <f aca="false">D55-C55</f>
+        <v>520</v>
+      </c>
       <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="15" t="str">
+      <c r="G55" s="14" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H55" s="15" t="n">
         <f aca="false">IF(AND(E55&lt;&gt;0,G55&lt;&gt;0),E55/G55,"")</f>
-        <v/>
+        <v>65000</v>
       </c>
       <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
+      <c r="J55" s="14" t="s">
+        <v>112</v>
+      </c>
       <c r="K55" s="14"/>
       <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="19"/>
+      <c r="M55" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N55" s="14" t="n">
+        <v>2024</v>
+      </c>
+      <c r="O55" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="14"/>
@@ -5539,6 +5559,7 @@
     <hyperlink ref="O52" r:id="rId50" display="Zhang, Z.; Huang, B.; Zhang, Z.; Chen, H. On-Chip Reconstructive Spectrometer Based on Parallel Cascaded Micro-Ring Resonators. Appl. Sci. 2024, 14, 4886. https://doi.org/10.3390/app14114886"/>
     <hyperlink ref="O53" r:id="rId51" display="Li A, Wu YF, Wang C et al. An inversely designed integrated spectrometer with reconfigurable performance and ultra-low power consumption. Opto-Electron Adv 7, 240099 (2024). doi: 10.29026/oea.2024.240099"/>
     <hyperlink ref="O54" r:id="rId52" display="Tian, M., Liu, B., Lu, Z. et al. Miniaturized on-chip spectrometer enabled by electrochromic modulation. Light Sci Appl 13, 278 (2024). https://doi.org/10.1038/s41377-024-01638-4"/>
+    <hyperlink ref="O55" r:id="rId53" location="ref-CR53" display="Yao, C., Zhang, W., Bao, P. et al. Chip-scale sensor for spectroscopic metrology. Nat Commun 15, 10305 (2024). https://doi.org/10.1038/s41467-024-54708-x"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5561,7 +5582,7 @@
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.86"/>
@@ -5589,13 +5610,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>6</v>
@@ -5604,28 +5625,28 @@
         <v>7</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>13</v>
@@ -5634,12 +5655,12 @@
         <v>14</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B3" s="28" t="n">
         <v>720</v>
@@ -5662,12 +5683,12 @@
         <v>1991</v>
       </c>
       <c r="P3" s="30" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B4" s="32" t="n">
         <v>400</v>
@@ -5698,12 +5719,12 @@
         <v>2021</v>
       </c>
       <c r="P4" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="32" t="n">
@@ -5722,7 +5743,7 @@
       <c r="J5" s="33"/>
       <c r="L5" s="32"/>
       <c r="M5" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="N5" s="32" t="s">
         <v>17</v>
@@ -5731,7 +5752,7 @@
         <v>2014</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
@@ -5756,7 +5777,7 @@
       <c r="J6" s="33"/>
       <c r="K6" s="32"/>
       <c r="M6" s="32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="N6" s="32" t="s">
         <v>17</v>
@@ -5765,7 +5786,7 @@
         <v>2019</v>
       </c>
       <c r="P6" s="36" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5783,13 +5804,13 @@
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
       <c r="H7" s="33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I7" s="33"/>
       <c r="J7" s="33"/>
       <c r="L7" s="32"/>
       <c r="M7" s="32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N7" s="32" t="s">
         <v>17</v>
@@ -5798,7 +5819,7 @@
         <v>2020</v>
       </c>
       <c r="P7" s="37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
@@ -5817,7 +5838,7 @@
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I8" s="33"/>
       <c r="J8" s="33"/>
@@ -5833,12 +5854,12 @@
         <v>2011</v>
       </c>
       <c r="P8" s="36" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B9" s="32" t="n">
         <v>300</v>
@@ -5852,16 +5873,16 @@
       <c r="E9" s="32"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H9" s="33" t="n">
         <v>25</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K9" s="32" t="n">
         <v>100</v>
@@ -5873,12 +5894,12 @@
         <v>2009</v>
       </c>
       <c r="P9" s="34" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B10" s="32" t="n">
         <v>350</v>
@@ -5892,13 +5913,13 @@
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H10" s="33" t="n">
         <v>30</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J10" s="33" t="n">
         <v>-2</v>
@@ -5915,12 +5936,12 @@
         <v>2013</v>
       </c>
       <c r="P10" s="34" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B11" s="32" t="n">
         <v>300</v>
@@ -5934,13 +5955,13 @@
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H11" s="33" t="n">
         <v>40</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J11" s="33" t="n">
         <v>-6</v>
@@ -5957,12 +5978,12 @@
         <v>2013</v>
       </c>
       <c r="P11" s="34" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B12" s="32" t="n">
         <v>300</v>
@@ -5976,13 +5997,13 @@
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H12" s="33" t="n">
         <v>70</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J12" s="33" t="n">
         <v>-1</v>
@@ -5999,12 +6020,12 @@
         <v>2014</v>
       </c>
       <c r="P12" s="34" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B13" s="32" t="n">
         <v>400</v>
@@ -6018,13 +6039,13 @@
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
       <c r="G13" s="32" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H13" s="33" t="n">
         <v>76</v>
       </c>
       <c r="I13" s="33" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J13" s="33" t="n">
         <v>-5</v>
@@ -6041,12 +6062,12 @@
         <v>2015</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B14" s="32" t="n">
         <v>610</v>
@@ -6062,13 +6083,13 @@
         <v>85</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H14" s="33" t="n">
         <v>35</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J14" s="33" t="n">
         <v>-1</v>
@@ -6085,12 +6106,12 @@
         <v>2015</v>
       </c>
       <c r="P14" s="34" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B15" s="32" t="n">
         <v>300</v>
@@ -6104,16 +6125,16 @@
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
       <c r="G15" s="32" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H15" s="33" t="n">
         <v>28</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K15" s="32" t="n">
         <v>148</v>
@@ -6127,12 +6148,12 @@
         <v>2015</v>
       </c>
       <c r="P15" s="34" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B16" s="32" t="n">
         <v>600</v>
@@ -6146,13 +6167,13 @@
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H16" s="33" t="n">
         <v>23</v>
       </c>
       <c r="I16" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J16" s="33" t="n">
         <v>-2</v>
@@ -6167,12 +6188,12 @@
         <v>2015</v>
       </c>
       <c r="P16" s="34" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B17" s="32" t="n">
         <v>900</v>
@@ -6188,13 +6209,13 @@
         <v>80</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="I17" s="33" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J17" s="33" t="n">
         <v>-1</v>
@@ -6207,12 +6228,12 @@
         <v>2015</v>
       </c>
       <c r="P17" s="34" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="31" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B18" s="32" t="n">
         <v>300</v>
@@ -6226,13 +6247,13 @@
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="G18" s="32" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H18" s="33" t="n">
         <v>27</v>
       </c>
       <c r="I18" s="33" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J18" s="33" t="n">
         <v>-2</v>
@@ -6249,12 +6270,12 @@
         <v>2016</v>
       </c>
       <c r="P18" s="34" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B19" s="32" t="n">
         <v>650</v>
@@ -6270,13 +6291,13 @@
         <v>100</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H19" s="33" t="n">
         <v>200</v>
       </c>
       <c r="I19" s="33" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J19" s="33" t="n">
         <v>-6</v>
@@ -6293,12 +6314,12 @@
         <v>2016</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="31" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" s="32" t="n">
         <v>640</v>
@@ -6314,7 +6335,7 @@
         <v>28</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H20" s="33" t="n">
         <v>53500</v>
@@ -6335,12 +6356,12 @@
         <v>2017</v>
       </c>
       <c r="P20" s="34" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B21" s="32" t="n">
         <v>700</v>
@@ -6356,13 +6377,13 @@
         <v>15</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H21" s="33" t="n">
         <v>40</v>
       </c>
       <c r="I21" s="33" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J21" s="33" t="n">
         <v>0</v>
@@ -6377,12 +6398,12 @@
         <v>2017</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B22" s="32" t="n">
         <v>700</v>
@@ -6398,13 +6419,13 @@
         <v>17</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H22" s="33" t="n">
         <v>24</v>
       </c>
       <c r="I22" s="33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J22" s="33" t="n">
         <v>0</v>
@@ -6419,12 +6440,12 @@
         <v>2017</v>
       </c>
       <c r="P22" s="34" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B23" s="32" t="n">
         <v>1000</v>
@@ -6440,13 +6461,13 @@
         <v>35</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I23" s="33" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J23" s="33" t="n">
         <v>0</v>
@@ -6459,12 +6480,12 @@
         <v>2017</v>
       </c>
       <c r="P23" s="34" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B24" s="32" t="n">
         <v>1000</v>
@@ -6480,13 +6501,13 @@
         <v>38</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="J24" s="33" t="n">
         <v>0</v>
@@ -6499,12 +6520,12 @@
         <v>2017</v>
       </c>
       <c r="P24" s="34" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="31" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B25" s="32" t="n">
         <v>1000</v>
@@ -6520,13 +6541,13 @@
         <v>47</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I25" s="33" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J25" s="33" t="n">
         <v>0</v>
@@ -6539,12 +6560,12 @@
         <v>2017</v>
       </c>
       <c r="P25" s="34" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="31" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B26" s="32" t="n">
         <v>1000</v>
@@ -6560,13 +6581,13 @@
         <v>41</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="J26" s="33" t="n">
         <v>0</v>
@@ -6579,12 +6600,12 @@
         <v>2017</v>
       </c>
       <c r="P26" s="34" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="31" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B27" s="32" t="n">
         <v>875</v>
@@ -6600,13 +6621,13 @@
         <v>43</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H27" s="33" t="n">
         <v>22</v>
       </c>
       <c r="I27" s="33" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J27" s="33" t="n">
         <v>0</v>
@@ -6621,12 +6642,12 @@
         <v>2017</v>
       </c>
       <c r="P27" s="34" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="31" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B28" s="32" t="n">
         <v>810</v>
@@ -6651,12 +6672,12 @@
         <v>2017</v>
       </c>
       <c r="P28" s="34" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="31" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B29" s="32" t="n">
         <v>400</v>
@@ -6670,13 +6691,13 @@
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
       <c r="G29" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H29" s="33" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I29" s="33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J29" s="33" t="n">
         <v>-40</v>
@@ -6691,12 +6712,12 @@
         <v>2018</v>
       </c>
       <c r="P29" s="34" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="31" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B30" s="32" t="n">
         <v>300</v>
@@ -6710,13 +6731,13 @@
       <c r="E30" s="32"/>
       <c r="F30" s="32"/>
       <c r="G30" s="32" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H30" s="33" t="n">
         <v>48</v>
       </c>
       <c r="I30" s="33" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J30" s="33" t="n">
         <v>0</v>
@@ -6729,12 +6750,12 @@
         <v>2018</v>
       </c>
       <c r="P30" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="31" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B31" s="32" t="n">
         <v>790</v>
@@ -6750,13 +6771,13 @@
         <v>30</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H31" s="33" t="n">
         <v>2000</v>
       </c>
       <c r="I31" s="33" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J31" s="33" t="n">
         <v>-50</v>
@@ -6771,12 +6792,12 @@
         <v>2018</v>
       </c>
       <c r="P31" s="34" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="31" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B32" s="32" t="n">
         <v>350</v>
@@ -6792,20 +6813,20 @@
         <v>20</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H32" s="33" t="n">
         <v>2170</v>
       </c>
       <c r="I32" s="33" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J32" s="33" t="n">
         <v>-15</v>
       </c>
       <c r="K32" s="32"/>
       <c r="L32" s="32" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="M32" s="32"/>
       <c r="N32" s="32"/>
@@ -6813,12 +6834,12 @@
         <v>2018</v>
       </c>
       <c r="P32" s="34" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="31" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B33" s="32" t="n">
         <v>300</v>
@@ -6832,16 +6853,16 @@
       <c r="E33" s="32"/>
       <c r="F33" s="32"/>
       <c r="G33" s="32" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H33" s="33" t="n">
         <v>56</v>
       </c>
       <c r="I33" s="33" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J33" s="33" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K33" s="32" t="n">
         <v>97</v>
@@ -6855,12 +6876,12 @@
         <v>2019</v>
       </c>
       <c r="P33" s="34" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B34" s="32" t="n">
         <v>420</v>
@@ -6876,13 +6897,13 @@
         <v>76</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H34" s="33" t="n">
         <v>18</v>
       </c>
       <c r="I34" s="33" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J34" s="33" t="n">
         <v>0</v>
@@ -6895,12 +6916,12 @@
         <v>2019</v>
       </c>
       <c r="P34" s="34" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="31" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B35" s="32" t="n">
         <v>400</v>
@@ -6916,13 +6937,13 @@
         <v>84</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H35" s="33" t="n">
         <v>50</v>
       </c>
       <c r="I35" s="33" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J35" s="33" t="n">
         <v>0</v>
@@ -6939,12 +6960,12 @@
         <v>2019</v>
       </c>
       <c r="P35" s="34" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="31" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B36" s="32" t="n">
         <v>810</v>
@@ -6960,13 +6981,13 @@
         <v>50</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J36" s="33" t="n">
         <v>0</v>
@@ -6979,12 +7000,12 @@
         <v>2019</v>
       </c>
       <c r="P36" s="38" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="31" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B37" s="32" t="n">
         <v>810</v>
@@ -7000,13 +7021,13 @@
         <v>50</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="J37" s="33" t="n">
         <v>0</v>
@@ -7019,12 +7040,12 @@
         <v>2019</v>
       </c>
       <c r="P37" s="38" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="31" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B38" s="32" t="n">
         <v>300</v>
@@ -7038,13 +7059,13 @@
       <c r="E38" s="32"/>
       <c r="F38" s="32"/>
       <c r="G38" s="32" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J38" s="33" t="n">
         <v>-2</v>
@@ -7053,7 +7074,7 @@
         <v>173</v>
       </c>
       <c r="L38" s="32" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="M38" s="32"/>
       <c r="N38" s="32"/>
@@ -7061,12 +7082,12 @@
         <v>2020</v>
       </c>
       <c r="P38" s="34" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="31" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B39" s="32" t="n">
         <v>645</v>
@@ -7082,13 +7103,13 @@
         <v>50</v>
       </c>
       <c r="G39" s="32" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H39" s="33" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I39" s="33" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J39" s="33" t="n">
         <v>0</v>
@@ -7097,7 +7118,7 @@
         <v>103</v>
       </c>
       <c r="L39" s="32" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="M39" s="32"/>
       <c r="N39" s="32"/>
@@ -7105,12 +7126,12 @@
         <v>2020</v>
       </c>
       <c r="P39" s="34" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="31" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B40" s="32" t="n">
         <v>860</v>
@@ -7126,16 +7147,16 @@
         <v>50</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H40" s="33" t="n">
         <v>61</v>
       </c>
       <c r="I40" s="33" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J40" s="33" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K40" s="32"/>
       <c r="L40" s="32"/>
@@ -7145,12 +7166,12 @@
         <v>2020</v>
       </c>
       <c r="P40" s="34" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B41" s="32" t="n">
         <v>860</v>
@@ -7166,12 +7187,12 @@
         <v>40</v>
       </c>
       <c r="G41" s="32" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
       <c r="J41" s="33" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K41" s="32"/>
       <c r="L41" s="32"/>
@@ -7181,12 +7202,12 @@
         <v>2020</v>
       </c>
       <c r="P41" s="34" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="31" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B42" s="32" t="n">
         <v>860</v>
@@ -7202,12 +7223,12 @@
         <v>50</v>
       </c>
       <c r="G42" s="32" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
       <c r="J42" s="33" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K42" s="32"/>
       <c r="L42" s="32"/>
@@ -7217,12 +7238,12 @@
         <v>2020</v>
       </c>
       <c r="P42" s="34" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B43" s="32" t="n">
         <v>750</v>
@@ -7238,13 +7259,13 @@
         <v>120</v>
       </c>
       <c r="G43" s="32" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H43" s="33" t="n">
         <v>53</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J43" s="33" t="n">
         <v>0</v>
@@ -7259,12 +7280,12 @@
         <v>2020</v>
       </c>
       <c r="P43" s="34" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B44" s="32" t="n">
         <v>790</v>
@@ -7280,13 +7301,13 @@
         <v>37</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H44" s="33" t="n">
         <v>10</v>
       </c>
       <c r="I44" s="33" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="J44" s="33" t="n">
         <v>0</v>
@@ -7301,12 +7322,12 @@
         <v>2020</v>
       </c>
       <c r="P44" s="34" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="31" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B45" s="32" t="n">
         <v>1020</v>
@@ -7322,13 +7343,13 @@
         <v>58</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H45" s="33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I45" s="33" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J45" s="33" t="n">
         <v>0</v>
@@ -7343,12 +7364,12 @@
         <v>2020</v>
       </c>
       <c r="P45" s="34" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="31" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B46" s="32" t="n">
         <v>300</v>
@@ -7362,16 +7383,16 @@
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H46" s="33" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I46" s="33" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J46" s="33" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K46" s="32" t="n">
         <v>123</v>
@@ -7385,12 +7406,12 @@
         <v>2021</v>
       </c>
       <c r="P46" s="34" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="31" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B47" s="32" t="n">
         <v>830</v>
@@ -7406,7 +7427,7 @@
         <v>27</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="H47" s="33" t="n">
         <v>15300</v>
@@ -7427,12 +7448,12 @@
         <v>2021</v>
       </c>
       <c r="P47" s="34" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="31" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B48" s="32" t="n">
         <v>650</v>
@@ -7448,13 +7469,13 @@
         <v>60</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H48" s="33" t="n">
         <v>18</v>
       </c>
       <c r="I48" s="33" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J48" s="33" t="n">
         <v>0</v>
@@ -7469,12 +7490,12 @@
         <v>2021</v>
       </c>
       <c r="P48" s="34" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="31" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B49" s="32" t="n">
         <v>650</v>
@@ -7490,13 +7511,13 @@
         <v>45</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H49" s="33" t="n">
         <v>6</v>
       </c>
       <c r="I49" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="J49" s="33" t="n">
         <v>0</v>
@@ -7509,12 +7530,12 @@
         <v>2021</v>
       </c>
       <c r="P49" s="34" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="31" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B50" s="32" t="n">
         <v>650</v>
@@ -7530,13 +7551,13 @@
         <v>35</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="H50" s="33" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="I50" s="33" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="J50" s="33" t="n">
         <v>0</v>
@@ -7549,12 +7570,12 @@
         <v>2021</v>
       </c>
       <c r="P50" s="34" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="31" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B51" s="32" t="n">
         <v>650</v>
@@ -7570,13 +7591,13 @@
         <v>20</v>
       </c>
       <c r="G51" s="32" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="H51" s="33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I51" s="33" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="J51" s="33" t="n">
         <v>0</v>
@@ -7589,12 +7610,12 @@
         <v>2021</v>
       </c>
       <c r="P51" s="34" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="31" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B52" s="32" t="n">
         <v>826</v>
@@ -7610,20 +7631,20 @@
         <v>17</v>
       </c>
       <c r="G52" s="32" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H52" s="33" t="n">
         <v>75</v>
       </c>
       <c r="I52" s="33" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="J52" s="33" t="n">
         <v>-10</v>
       </c>
       <c r="K52" s="32"/>
       <c r="L52" s="32" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M52" s="32"/>
       <c r="N52" s="32"/>
@@ -7631,7 +7652,7 @@
         <v>2021</v>
       </c>
       <c r="P52" s="34" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8057,7 +8078,7 @@
       <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.14"/>
@@ -8066,13 +8087,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8122,13 +8143,13 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
       <c r="B8" s="39" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39"/>
       <c r="B9" s="41" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8146,7 +8167,7 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="39"/>
       <c r="B12" s="39" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8158,7 +8179,7 @@
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="39"/>
       <c r="B14" s="39" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8170,277 +8191,277 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
       <c r="B16" s="39" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39"/>
       <c r="B17" s="39" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
       <c r="B18" s="39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="39"/>
       <c r="B19" s="39" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
       <c r="B20" s="39" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
       <c r="B21" s="39" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="39"/>
       <c r="B22" s="39" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="39"/>
       <c r="B23" s="39" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="39"/>
       <c r="B24" s="39" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="39"/>
       <c r="B25" s="39" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
       <c r="B26" s="39" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39"/>
       <c r="B27" s="39" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="39"/>
       <c r="B28" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="39"/>
       <c r="B29" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="39"/>
       <c r="B31" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="39"/>
       <c r="B32" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="39"/>
       <c r="B33" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="39"/>
       <c r="B34" s="39" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="39"/>
       <c r="B35" s="39" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="39"/>
       <c r="B36" s="39" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="39"/>
       <c r="B37" s="39" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="39"/>
       <c r="B38" s="39" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="39"/>
       <c r="B39" s="39" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="39"/>
       <c r="B40" s="39" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="39"/>
       <c r="B41" s="39" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="39"/>
       <c r="B42" s="39" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="39"/>
       <c r="B43" s="39" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="39"/>
       <c r="B44" s="39" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="39"/>
       <c r="B45" s="39" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="39"/>
       <c r="B46" s="39" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="39"/>
       <c r="B47" s="39" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="39"/>
       <c r="B48" s="39" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="39"/>
       <c r="B49" s="39" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="39"/>
       <c r="B50" s="39" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="39"/>
       <c r="B51" s="39" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="39"/>
       <c r="B52" s="39" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="39"/>
       <c r="B53" s="39" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="39"/>
       <c r="B54" s="39" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="39"/>
       <c r="B55" s="39" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="39"/>
       <c r="B56" s="39" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="39"/>
       <c r="B57" s="39" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="39"/>
       <c r="B58" s="39" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="39"/>
       <c r="B59" s="39" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="39"/>
       <c r="B60" s="39" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="39"/>
       <c r="B61" s="42" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add type for yao et al. 2024 Chip-scale sensor for spectroscopic metrology
</commit_message>
<xml_diff>
--- a/iPHAOS.xlsx
+++ b/iPHAOS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="285">
   <si>
     <t xml:space="preserve">Spectral range</t>
   </si>
@@ -1005,11 +1005,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
-    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -1337,7 +1336,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1497,8 +1496,8 @@
   </sheetPr>
   <dimension ref="A1:O268"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O13" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O57" activeCellId="0" sqref="O57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3577,7 +3576,9 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14"/>
+      <c r="A55" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="B55" s="14" t="s">
         <v>24</v>
       </c>

</xml_diff>